<commit_message>
added student report, report ui and contrller classes
Signed-off-by: yajatgulati <yajatgulati01@gmail.com>
</commit_message>
<xml_diff>
--- a/camp_participants.xlsx
+++ b/camp_participants.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -449,6 +449,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C4" t="n" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="D4" t="n" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E4" t="b" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>